<commit_message>
Before Add Test Case
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kudzi\source\repos\UiPath\UiPath-REFramework-Project-with-Tabular-Data\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AF7B21-74C7-4564-92B5-3BA1744F4A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C91E7C4-0BE5-4D38-A963-2EC699A36600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25935" yWindow="2640" windowWidth="24975" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21255" yWindow="4200" windowWidth="24975" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>ManualTransactionTreshold</t>
+  </si>
+  <si>
+    <t>StatusFilePath</t>
+  </si>
+  <si>
+    <t>Data\Output\Status.xlsx</t>
   </si>
 </sst>
 </file>
@@ -541,7 +547,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -632,7 +638,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>